<commit_message>
info added in excel
</commit_message>
<xml_diff>
--- a/Devops learners.xlsx
+++ b/Devops learners.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devopslearners\Update_XL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/138a9cedd38fcb68/Documents/devopslearner/devopslearners/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F106A5-D3FF-4DF5-8954-4B85611CE003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E2F106A5-D3FF-4DF5-8954-4B85611CE003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{896E03B5-1CD6-43D9-8C8B-DD8F203096C1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24315" yWindow="1230" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Manual Tester</t>
+  </si>
+  <si>
+    <t>jatin bhalla</t>
+  </si>
+  <si>
+    <t>jatinbhalla18@gmail.com</t>
+  </si>
+  <si>
+    <t>Devops engineer</t>
   </si>
 </sst>
 </file>
@@ -417,20 +426,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="41.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -455,7 +464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -464,12 +473,24 @@
       </c>
       <c r="C3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{D5BE6B78-96EC-4FFC-8C2C-5D47B9806D11}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{B36ABC57-C157-4A4C-A68B-7B6CE6300617}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New DevOps added in excel
</commit_message>
<xml_diff>
--- a/Devops learners.xlsx
+++ b/Devops learners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishesh Pandey\devopslearners\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2CC62D-9EC6-4B80-8E4F-3C01BC21DDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B32D1F4-5F4B-4717-BDFB-FF7B0BCB8599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,13 +66,13 @@
     <t>Devops engineer</t>
   </si>
   <si>
-    <t>Vishesh Pandey</t>
-  </si>
-  <si>
     <t>visheshpandey0@gmail.com</t>
   </si>
   <si>
     <t>Java Developer</t>
+  </si>
+  <si>
+    <t>vishesh pandey</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,13 +497,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>